<commit_message>
modified getting item info functionality, added narrator implementation notebook
</commit_message>
<xml_diff>
--- a/DnD.xlsx
+++ b/DnD.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HSW\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/662b58f4f53a6bab/Work/Masters/W210/ll-dm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768AF4F0-FA2C-47C2-A03E-14FF70387FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{768AF4F0-FA2C-47C2-A03E-14FF70387FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F608C6F6-120E-40EE-8122-B8D4D95FD729}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="756" activeTab="1" xr2:uid="{BA24B464-A3E7-4082-BD8F-2FE131915583}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="50910" windowHeight="21840" tabRatio="756" activeTab="2" xr2:uid="{BA24B464-A3E7-4082-BD8F-2FE131915583}"/>
   </bookViews>
   <sheets>
     <sheet name="Character sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Inventory" sheetId="2" r:id="rId2"/>
-    <sheet name="Settings" sheetId="7" r:id="rId3"/>
-    <sheet name="NPCs" sheetId="9" r:id="rId4"/>
-    <sheet name="Treasures" sheetId="8" r:id="rId5"/>
-    <sheet name="Monsters" sheetId="4" r:id="rId6"/>
-    <sheet name="Plot" sheetId="6" r:id="rId7"/>
-    <sheet name="Logs" sheetId="5" r:id="rId8"/>
+    <sheet name="World Items" sheetId="10" r:id="rId3"/>
+    <sheet name="Settings" sheetId="7" r:id="rId4"/>
+    <sheet name="NPCs" sheetId="9" r:id="rId5"/>
+    <sheet name="Treasures" sheetId="8" r:id="rId6"/>
+    <sheet name="Monsters" sheetId="4" r:id="rId7"/>
+    <sheet name="Plot" sheetId="6" r:id="rId8"/>
+    <sheet name="Logs" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="420">
   <si>
     <t>Name</t>
   </si>
@@ -429,26 +430,919 @@
   </si>
   <si>
     <t>A sturdy brown mare for reliable transportation.</t>
+  </si>
+  <si>
+    <t>Weapon Name</t>
+  </si>
+  <si>
+    <t>Weapon Description</t>
+  </si>
+  <si>
+    <t>Prompt</t>
+  </si>
+  <si>
+    <t>Legendary Wand of Assassin</t>
+  </si>
+  <si>
+    <t>The Legendary Wand of Assassin is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Wand of Assassin in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Lance of Knight</t>
+  </si>
+  <si>
+    <t>The Forgotten Lance of Knight is a lance known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this lance is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Lance of Knight in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Cursed Armor of Warrior</t>
+  </si>
+  <si>
+    <t>The Cursed Armor of Warrior is a armor known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this armor is imbued with the essence of ranger. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Cursed Armor of Warrior in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Divine Bow of Ranger</t>
+  </si>
+  <si>
+    <t>The Divine Bow of Ranger is a bow known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bow is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Divine Bow of Ranger in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Cursed Armor of Storm</t>
+  </si>
+  <si>
+    <t>The Cursed Armor of Storm is a armor known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this armor is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Cursed Armor of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Ancient Axe of Warrior</t>
+  </si>
+  <si>
+    <t>The Ancient Axe of Warrior is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Ancient Axe of Warrior in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Mystic Axe of Ranger</t>
+  </si>
+  <si>
+    <t>The Mystic Axe of Ranger is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Mystic Axe of Ranger in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Wand of Frost</t>
+  </si>
+  <si>
+    <t>The Forgotten Wand of Frost is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Wand of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Ancient Armor of Phoenix</t>
+  </si>
+  <si>
+    <t>The Ancient Armor of Phoenix is a armor known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this armor is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Ancient Armor of Phoenix in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Divine Ring of Frost</t>
+  </si>
+  <si>
+    <t>The Divine Ring of Frost is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of knight. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Divine Ring of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Arcane Axe of Warrior</t>
+  </si>
+  <si>
+    <t>The Arcane Axe of Warrior is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Arcane Axe of Warrior in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Shadow Armor of Knight</t>
+  </si>
+  <si>
+    <t>The Shadow Armor of Knight is a armor known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this armor is imbued with the essence of storm. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Armor of Knight in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Cursed Sword of Ranger</t>
+  </si>
+  <si>
+    <t>The Cursed Sword of Ranger is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Cursed Sword of Ranger in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Glowing Sword of Warrior</t>
+  </si>
+  <si>
+    <t>The Glowing Sword of Warrior is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Glowing Sword of Warrior in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Ring of Mage</t>
+  </si>
+  <si>
+    <t>The Legendary Ring of Mage is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of warrior. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Ring of Mage in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>The Shadow Armor of Knight is a armor known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this armor is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Ancient Bow of Flame</t>
+  </si>
+  <si>
+    <t>The Ancient Bow of Flame is a bow known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bow is imbued with the essence of ranger. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Ancient Bow of Flame in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Divine Wand of Assassin</t>
+  </si>
+  <si>
+    <t>The Divine Wand of Assassin is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Divine Wand of Assassin in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Glowing Axe of Storm</t>
+  </si>
+  <si>
+    <t>The Glowing Axe of Storm is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of warrior. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Glowing Axe of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Shadow Armor of Ranger</t>
+  </si>
+  <si>
+    <t>The Shadow Armor of Ranger is a armor known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this armor is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Armor of Ranger in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Divine Axe of Warrior</t>
+  </si>
+  <si>
+    <t>The Divine Axe of Warrior is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Divine Axe of Warrior in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Helmet of Mage</t>
+  </si>
+  <si>
+    <t>The Forgotten Helmet of Mage is a helmet known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this helmet is imbued with the essence of knight. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Helmet of Mage in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Ring of Frost</t>
+  </si>
+  <si>
+    <t>The Legendary Ring of Frost is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Ring of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Bracelet of Frost</t>
+  </si>
+  <si>
+    <t>The Forgotten Bracelet of Frost is a bracelet known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bracelet is imbued with the essence of phoenix. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Bracelet of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Shadow Ring of Flame</t>
+  </si>
+  <si>
+    <t>The Shadow Ring of Flame is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of ranger. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Ring of Flame in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Sword of Ranger</t>
+  </si>
+  <si>
+    <t>The Legendary Sword of Ranger is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of assassin. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Sword of Ranger in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Shadow Sword of Warrior</t>
+  </si>
+  <si>
+    <t>The Shadow Sword of Warrior is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Sword of Warrior in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Armor of Assassin</t>
+  </si>
+  <si>
+    <t>The Legendary Armor of Assassin is a armor known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this armor is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Armor of Assassin in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Ancient Shoes of Storm</t>
+  </si>
+  <si>
+    <t>The Ancient Shoes of Storm is a shoes known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this shoes is imbued with the essence of ranger. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Ancient Shoes of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Wand of Flame</t>
+  </si>
+  <si>
+    <t>The Legendary Wand of Flame is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Wand of Flame in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Shadow Shoes of Storm</t>
+  </si>
+  <si>
+    <t>The Shadow Shoes of Storm is a shoes known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this shoes is imbued with the essence of phoenix. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Shoes of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Mystic Shoes of Storm</t>
+  </si>
+  <si>
+    <t>The Mystic Shoes of Storm is a shoes known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this shoes is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Mystic Shoes of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Ancient Wand of Phoenix</t>
+  </si>
+  <si>
+    <t>The Ancient Wand of Phoenix is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of storm. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Ancient Wand of Phoenix in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Divine Ring of Flame</t>
+  </si>
+  <si>
+    <t>The Divine Ring of Flame is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of warrior. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Divine Ring of Flame in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Ring of Knight</t>
+  </si>
+  <si>
+    <t>The Legendary Ring of Knight is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Ring of Knight in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Enchanted Wand of Storm</t>
+  </si>
+  <si>
+    <t>The Enchanted Wand of Storm is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of knight. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Enchanted Wand of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Enchanted Axe of Frost</t>
+  </si>
+  <si>
+    <t>The Enchanted Axe of Frost is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Enchanted Axe of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Mystic Ring of Mage</t>
+  </si>
+  <si>
+    <t>The Mystic Ring of Mage is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of ranger. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Mystic Ring of Mage in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Mystic Shoes of Frost</t>
+  </si>
+  <si>
+    <t>The Mystic Shoes of Frost is a shoes known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this shoes is imbued with the essence of storm. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Mystic Shoes of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Glowing Sword of Mage</t>
+  </si>
+  <si>
+    <t>The Glowing Sword of Mage is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Glowing Sword of Mage in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Glowing Shoes of Ranger</t>
+  </si>
+  <si>
+    <t>The Glowing Shoes of Ranger is a shoes known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this shoes is imbued with the essence of ranger. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Glowing Shoes of Ranger in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Ancient Sword of Warrior</t>
+  </si>
+  <si>
+    <t>The Ancient Sword of Warrior is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of knight. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Ancient Sword of Warrior in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Shadow Axe of Frost</t>
+  </si>
+  <si>
+    <t>The Shadow Axe of Frost is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Axe of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Arcane Shoes of Assassin</t>
+  </si>
+  <si>
+    <t>The Arcane Shoes of Assassin is a shoes known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this shoes is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Arcane Shoes of Assassin in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Divine Bracelet of Ranger</t>
+  </si>
+  <si>
+    <t>The Divine Bracelet of Ranger is a bracelet known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bracelet is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Divine Bracelet of Ranger in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Ancient Bow of Phoenix</t>
+  </si>
+  <si>
+    <t>The Ancient Bow of Phoenix is a bow known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bow is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Ancient Bow of Phoenix in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Lance of Storm</t>
+  </si>
+  <si>
+    <t>The Forgotten Lance of Storm is a lance known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this lance is imbued with the essence of storm. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Lance of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Shadow Shoes of Knight</t>
+  </si>
+  <si>
+    <t>The Shadow Shoes of Knight is a shoes known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this shoes is imbued with the essence of phoenix. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Shoes of Knight in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Lance of Warrior</t>
+  </si>
+  <si>
+    <t>The Forgotten Lance of Warrior is a lance known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this lance is imbued with the essence of phoenix. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Lance of Warrior in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Armor of Mage</t>
+  </si>
+  <si>
+    <t>The Legendary Armor of Mage is a armor known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this armor is imbued with the essence of knight. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Armor of Mage in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Bracelet of Assassin</t>
+  </si>
+  <si>
+    <t>The Forgotten Bracelet of Assassin is a bracelet known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bracelet is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Bracelet of Assassin in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Enchanted Sword of Storm</t>
+  </si>
+  <si>
+    <t>The Enchanted Sword of Storm is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Enchanted Sword of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>The Mystic Ring of Mage is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Arcane Ring of Assassin</t>
+  </si>
+  <si>
+    <t>The Arcane Ring of Assassin is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of warrior. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Arcane Ring of Assassin in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Ancient Sword of Knight</t>
+  </si>
+  <si>
+    <t>The Ancient Sword of Knight is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of phoenix. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Ancient Sword of Knight in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>The Forgotten Helmet of Mage is a helmet known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this helmet is imbued with the essence of ranger. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Shadow Axe of Flame</t>
+  </si>
+  <si>
+    <t>The Shadow Axe of Flame is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Axe of Flame in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Sword of Frost</t>
+  </si>
+  <si>
+    <t>The Legendary Sword of Frost is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Sword of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Sword of Knight</t>
+  </si>
+  <si>
+    <t>The Forgotten Sword of Knight is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of phoenix. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Sword of Knight in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Cursed Ring of Assassin</t>
+  </si>
+  <si>
+    <t>The Cursed Ring of Assassin is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Cursed Ring of Assassin in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Cursed Ring of Mage</t>
+  </si>
+  <si>
+    <t>The Cursed Ring of Mage is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Cursed Ring of Mage in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Shadow Belt of Storm</t>
+  </si>
+  <si>
+    <t>The Shadow Belt of Storm is a belt known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this belt is imbued with the essence of ranger. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Belt of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Helmet of Ranger</t>
+  </si>
+  <si>
+    <t>The Legendary Helmet of Ranger is a helmet known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this helmet is imbued with the essence of warrior. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Helmet of Ranger in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Enchanted Shoes of Ranger</t>
+  </si>
+  <si>
+    <t>The Enchanted Shoes of Ranger is a shoes known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this shoes is imbued with the essence of assassin. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Enchanted Shoes of Ranger in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Ring of Flame</t>
+  </si>
+  <si>
+    <t>The Forgotten Ring of Flame is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of storm. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Ring of Flame in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Enchanted Wand of Knight</t>
+  </si>
+  <si>
+    <t>The Enchanted Wand of Knight is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Enchanted Wand of Knight in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Armor of Frost</t>
+  </si>
+  <si>
+    <t>The Legendary Armor of Frost is a armor known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this armor is imbued with the essence of storm. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Armor of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Mystic Sword of Mage</t>
+  </si>
+  <si>
+    <t>The Mystic Sword of Mage is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Mystic Sword of Mage in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Glowing Ring of Assassin</t>
+  </si>
+  <si>
+    <t>The Glowing Ring of Assassin is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Glowing Ring of Assassin in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Mystic Wand of Dragon</t>
+  </si>
+  <si>
+    <t>The Mystic Wand of Dragon is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Mystic Wand of Dragon in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Glowing Lance of Phoenix</t>
+  </si>
+  <si>
+    <t>The Glowing Lance of Phoenix is a lance known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this lance is imbued with the essence of knight. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Glowing Lance of Phoenix in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Mystic Ring of Knight</t>
+  </si>
+  <si>
+    <t>The Mystic Ring of Knight is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of phoenix. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Mystic Ring of Knight in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Mystic Axe of Phoenix</t>
+  </si>
+  <si>
+    <t>The Mystic Axe of Phoenix is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of knight. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Mystic Axe of Phoenix in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Ancient Bow of Warrior</t>
+  </si>
+  <si>
+    <t>The Ancient Bow of Warrior is a bow known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bow is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Ancient Bow of Warrior in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Mystic Lance of Mage</t>
+  </si>
+  <si>
+    <t>The Mystic Lance of Mage is a lance known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this lance is imbued with the essence of phoenix. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Mystic Lance of Mage in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Arcane Bracelet of Phoenix</t>
+  </si>
+  <si>
+    <t>The Arcane Bracelet of Phoenix is a bracelet known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bracelet is imbued with the essence of knight. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Arcane Bracelet of Phoenix in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Cursed Wand of Assassin</t>
+  </si>
+  <si>
+    <t>The Cursed Wand of Assassin is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of ranger. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Cursed Wand of Assassin in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Cursed Shoes of Dragon</t>
+  </si>
+  <si>
+    <t>The Cursed Shoes of Dragon is a shoes known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this shoes is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Cursed Shoes of Dragon in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Arcane Lance of Dragon</t>
+  </si>
+  <si>
+    <t>The Arcane Lance of Dragon is a lance known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this lance is imbued with the essence of assassin. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Arcane Lance of Dragon in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Glowing Axe of Ranger</t>
+  </si>
+  <si>
+    <t>The Glowing Axe of Ranger is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of assassin. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Glowing Axe of Ranger in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Mystic Wand of Knight</t>
+  </si>
+  <si>
+    <t>The Mystic Wand of Knight is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Mystic Wand of Knight in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Shoes of Storm</t>
+  </si>
+  <si>
+    <t>The Forgotten Shoes of Storm is a shoes known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this shoes is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Shoes of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Armor of Storm</t>
+  </si>
+  <si>
+    <t>The Forgotten Armor of Storm is a armor known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this armor is imbued with the essence of dragon. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Armor of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Arcane Bow of Mage</t>
+  </si>
+  <si>
+    <t>The Arcane Bow of Mage is a bow known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bow is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Arcane Bow of Mage in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Shadow Wand of Assassin</t>
+  </si>
+  <si>
+    <t>The Shadow Wand of Assassin is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Wand of Assassin in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Axe of Warrior</t>
+  </si>
+  <si>
+    <t>The Legendary Axe of Warrior is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Axe of Warrior in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Enchanted Axe of Dragon</t>
+  </si>
+  <si>
+    <t>The Enchanted Axe of Dragon is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of knight. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Enchanted Axe of Dragon in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Arcane Belt of Frost</t>
+  </si>
+  <si>
+    <t>The Arcane Belt of Frost is a belt known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this belt is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Arcane Belt of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Mystic Sword of Frost</t>
+  </si>
+  <si>
+    <t>The Mystic Sword of Frost is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Mystic Sword of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Shadow Wand of Dragon</t>
+  </si>
+  <si>
+    <t>The Shadow Wand of Dragon is a wand known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this wand is imbued with the essence of ranger. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Wand of Dragon in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Arcane Ring of Frost</t>
+  </si>
+  <si>
+    <t>The Arcane Ring of Frost is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Arcane Ring of Frost in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Ancient Bow of Ranger</t>
+  </si>
+  <si>
+    <t>The Ancient Bow of Ranger is a bow known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bow is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Ancient Bow of Ranger in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Legendary Bow of Flame</t>
+  </si>
+  <si>
+    <t>The Legendary Bow of Flame is a bow known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bow is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Legendary Bow of Flame in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Enchanted Bow of Storm</t>
+  </si>
+  <si>
+    <t>The Enchanted Bow of Storm is a bow known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this bow is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Enchanted Bow of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Arcane Belt of Dragon</t>
+  </si>
+  <si>
+    <t>The Arcane Belt of Dragon is a belt known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this belt is imbued with the essence of storm. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Arcane Belt of Dragon in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Glowing Armor of Warrior</t>
+  </si>
+  <si>
+    <t>The Glowing Armor of Warrior is a armor known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this armor is imbued with the essence of warrior. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Glowing Armor of Warrior in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Divine Ring of Mage</t>
+  </si>
+  <si>
+    <t>The Divine Ring of Mage is a ring known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this ring is imbued with the essence of frost. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Divine Ring of Mage in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Shadow Lance of Storm</t>
+  </si>
+  <si>
+    <t>The Shadow Lance of Storm is a lance known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this lance is imbued with the essence of mage. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Shadow Lance of Storm in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>Forgotten Sword of Flame</t>
+  </si>
+  <si>
+    <t>The Forgotten Sword of Flame is a sword known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this sword is imbued with the essence of flame. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
+  </si>
+  <si>
+    <t>Describe the weapon named Forgotten Sword of Flame in detail, including its history, special abilities, and appearance.</t>
+  </si>
+  <si>
+    <t>The Mystic Axe of Phoenix is a axe known throughout the realms for its incredible power. Forged in the fires of an ancient forge, this axe is imbued with the essence of warrior. It is said that those who wield it gain unmatched abilities, making them formidable in any battle.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -460,12 +1354,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -474,13 +1383,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -496,7 +1409,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -818,9 +1731,9 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -867,7 +1780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -924,13 +1837,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0A2D3E-86D5-4362-B5FC-08DB35034A63}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -941,7 +1854,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -952,7 +1865,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -963,7 +1876,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -974,7 +1887,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -985,7 +1898,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -996,7 +1909,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -1007,7 +1920,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -1018,7 +1931,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -1029,7 +1942,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -1040,7 +1953,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -1051,7 +1964,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>122</v>
       </c>
@@ -1069,6 +1982,1138 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0BDA4F-FC00-47EC-AC32-28690BB908B7}">
+  <dimension ref="A1:C101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="198.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35A6D33-7710-4A5E-8065-E528B10C51ED}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1076,9 +3121,9 @@
       <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1098,7 +3143,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1118,7 +3163,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1138,7 +3183,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1164,20 +3209,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F009F05-CB8B-46BC-B7FA-EEE0BFDBCB81}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528335C9-C6AA-4940-B113-2F7B37AECF07}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1185,9 +3230,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1210,7 +3255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -1239,7 +3284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283925CA-1F4D-4BC6-AA3C-CA7BF5C301F8}">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -1247,9 +3292,9 @@
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1317,7 +3362,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1391,7 +3436,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C9F4C7-5EB0-4E27-B585-F0B461004D8A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1399,9 +3444,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1412,7 +3457,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -1423,7 +3468,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -1434,7 +3479,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -1451,7 +3496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87D7DD1-D982-4380-B077-5010BE64F82E}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1459,9 +3504,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>73</v>
       </c>

</xml_diff>